<commit_message>
Update Tee config tools
</commit_message>
<xml_diff>
--- a/Tee System/TeeConfig.xlsx
+++ b/Tee System/TeeConfig.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fotoable/Gamedev_Tools/Tee System/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB25C63-2D76-484B-8E7A-E671C462CEC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50634379-CFC6-FB45-9537-73336D83F4FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-2500" yWindow="-21600" windowWidth="19060" windowHeight="21600" xr2:uid="{AE8D959E-CB57-7841-B8F1-A546B7A0C952}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="46">
   <si>
     <t>Notes</t>
   </si>
@@ -58,9 +58,6 @@
     <t>buff_list</t>
   </si>
   <si>
-    <t>condition</t>
-  </si>
-  <si>
     <t>extra_trophy</t>
   </si>
   <si>
@@ -161,13 +158,28 @@
   </si>
   <si>
     <t>Skill6_note</t>
+  </si>
+  <si>
+    <t>condition1</t>
+  </si>
+  <si>
+    <t>condition2</t>
+  </si>
+  <si>
+    <t>condition3</t>
+  </si>
+  <si>
+    <t>condition4</t>
+  </si>
+  <si>
+    <t>condition5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -177,6 +189,11 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="苹方-简"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="苹方-简"/>
       <family val="2"/>
     </font>
@@ -321,12 +338,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -667,8 +681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CB9F4E4-17F2-2041-B9BC-81AB44595C68}">
   <dimension ref="A1:V6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="T13" sqref="T13"/>
+    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -677,12 +691,12 @@
     <col min="7" max="7" width="17.5703125" customWidth="1"/>
     <col min="8" max="9" width="8" customWidth="1"/>
     <col min="10" max="10" width="7.85546875" customWidth="1"/>
-    <col min="11" max="12" width="10.7109375" style="16"/>
-    <col min="13" max="14" width="10.7109375" style="17"/>
-    <col min="15" max="16" width="10.7109375" style="18"/>
-    <col min="17" max="18" width="10.7109375" style="19"/>
-    <col min="19" max="20" width="10.7109375" style="20"/>
-    <col min="21" max="22" width="10.7109375" style="22"/>
+    <col min="11" max="12" width="10.7109375" style="15"/>
+    <col min="13" max="14" width="10.7109375" style="16"/>
+    <col min="15" max="16" width="10.7109375" style="17"/>
+    <col min="17" max="18" width="10.7109375" style="18"/>
+    <col min="19" max="20" width="10.7109375" style="19"/>
+    <col min="21" max="22" width="10.7109375" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22">
@@ -716,40 +730,40 @@
       <c r="J1">
         <v>10</v>
       </c>
-      <c r="K1" s="15">
+      <c r="K1" s="14">
         <v>11</v>
       </c>
-      <c r="L1" s="15">
+      <c r="L1" s="14">
         <v>12</v>
       </c>
-      <c r="M1" s="15">
+      <c r="M1" s="14">
         <v>13</v>
       </c>
-      <c r="N1" s="15">
+      <c r="N1" s="14">
         <v>14</v>
       </c>
-      <c r="O1" s="15">
+      <c r="O1" s="14">
         <v>15</v>
       </c>
-      <c r="P1" s="15">
+      <c r="P1" s="14">
         <v>16</v>
       </c>
-      <c r="Q1" s="15">
+      <c r="Q1" s="14">
         <v>17</v>
       </c>
-      <c r="R1" s="15">
+      <c r="R1" s="14">
         <v>18</v>
       </c>
-      <c r="S1" s="15">
+      <c r="S1" s="14">
         <v>19</v>
       </c>
-      <c r="T1" s="15">
+      <c r="T1" s="14">
         <v>20</v>
       </c>
-      <c r="U1" s="15">
+      <c r="U1" s="14">
         <v>21</v>
       </c>
-      <c r="V1" s="15">
+      <c r="V1" s="14">
         <v>22</v>
       </c>
     </row>
@@ -758,67 +772,67 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>22</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>23</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>24</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>25</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>26</v>
       </c>
-      <c r="I2" t="s">
-        <v>27</v>
-      </c>
       <c r="J2" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="K2" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="L2" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="L2" s="16" t="s">
+      <c r="M2" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="M2" s="17" t="s">
+      <c r="N2" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="N2" s="17" t="s">
+      <c r="O2" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="O2" s="18" t="s">
+      <c r="P2" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="P2" s="18" t="s">
+      <c r="Q2" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="Q2" s="19" t="s">
+      <c r="R2" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="R2" s="19" t="s">
+      <c r="S2" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="S2" s="20" t="s">
+      <c r="T2" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="T2" s="20" t="s">
+      <c r="U2" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="U2" s="21" t="s">
+      <c r="V2" s="20" t="s">
         <v>40</v>
-      </c>
-      <c r="V2" s="21" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:22">
@@ -1026,8 +1040,8 @@
       </c>
     </row>
     <row r="6" spans="1:22">
-      <c r="M6" s="17" t="s">
-        <v>28</v>
+      <c r="M6" s="16" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1037,289 +1051,838 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F412759-F70B-1343-9C94-8D49C9A91198}">
-  <dimension ref="A1:X8"/>
+  <dimension ref="A1:AV8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="AV16" sqref="AV16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
+  <cols>
+    <col min="1" max="1" width="27.5703125" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" customWidth="1"/>
+    <col min="10" max="11" width="9.85546875" customWidth="1"/>
+    <col min="12" max="12" width="10" customWidth="1"/>
+    <col min="13" max="13" width="9.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:48">
       <c r="A1">
         <v>1</v>
       </c>
-      <c r="C1" s="1">
-        <v>2</v>
+      <c r="B1">
+        <v>2</v>
+      </c>
+      <c r="C1">
+        <v>3</v>
       </c>
       <c r="D1">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1">
         <v>4</v>
       </c>
+      <c r="E1">
+        <v>5</v>
+      </c>
       <c r="F1">
+        <v>6</v>
+      </c>
+      <c r="G1">
+        <v>7</v>
+      </c>
+      <c r="H1">
+        <v>8</v>
+      </c>
+      <c r="I1">
+        <v>9</v>
+      </c>
+      <c r="J1">
+        <v>10</v>
+      </c>
+      <c r="K1">
+        <v>11</v>
+      </c>
+      <c r="L1">
+        <v>12</v>
+      </c>
+      <c r="M1">
+        <v>13</v>
+      </c>
+      <c r="N1">
+        <v>14</v>
+      </c>
+      <c r="O1">
+        <v>15</v>
+      </c>
+      <c r="P1">
+        <v>16</v>
+      </c>
+      <c r="Q1">
+        <v>17</v>
+      </c>
+      <c r="R1">
+        <v>18</v>
+      </c>
+      <c r="S1">
+        <v>19</v>
+      </c>
+      <c r="T1">
+        <v>20</v>
+      </c>
+      <c r="U1">
+        <v>21</v>
+      </c>
+      <c r="V1">
+        <v>22</v>
+      </c>
+      <c r="W1">
+        <v>23</v>
+      </c>
+      <c r="X1">
+        <v>24</v>
+      </c>
+      <c r="Y1">
+        <v>25</v>
+      </c>
+      <c r="Z1">
+        <v>26</v>
+      </c>
+      <c r="AA1">
+        <v>27</v>
+      </c>
+      <c r="AB1">
+        <v>28</v>
+      </c>
+      <c r="AC1">
+        <v>29</v>
+      </c>
+      <c r="AD1">
+        <v>30</v>
+      </c>
+      <c r="AE1">
+        <v>31</v>
+      </c>
+      <c r="AF1">
+        <v>32</v>
+      </c>
+      <c r="AG1">
+        <v>33</v>
+      </c>
+      <c r="AH1">
+        <v>34</v>
+      </c>
+      <c r="AI1">
+        <v>35</v>
+      </c>
+      <c r="AJ1">
+        <v>36</v>
+      </c>
+      <c r="AK1">
+        <v>37</v>
+      </c>
+      <c r="AL1">
+        <v>38</v>
+      </c>
+      <c r="AM1">
+        <v>39</v>
+      </c>
+      <c r="AN1">
+        <v>40</v>
+      </c>
+      <c r="AO1">
+        <v>41</v>
+      </c>
+      <c r="AP1">
+        <v>42</v>
+      </c>
+      <c r="AQ1">
+        <v>43</v>
+      </c>
+      <c r="AR1">
+        <v>44</v>
+      </c>
+      <c r="AS1">
+        <v>45</v>
+      </c>
+      <c r="AT1">
+        <v>46</v>
+      </c>
+      <c r="AU1">
+        <v>47</v>
+      </c>
+      <c r="AV1">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:48">
+      <c r="D2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
+      <c r="S2" s="12"/>
+      <c r="T2" s="12"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="12"/>
+      <c r="W2" s="12"/>
+      <c r="X2" s="12"/>
+      <c r="Y2" s="12"/>
+      <c r="Z2" s="12"/>
+      <c r="AA2" s="12"/>
+      <c r="AB2" s="12"/>
+    </row>
+    <row r="3" spans="1:48">
+      <c r="D3" s="1"/>
+      <c r="E3" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12"/>
+      <c r="S3" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="T3" s="13"/>
+      <c r="U3" s="13"/>
+      <c r="V3" s="13"/>
+      <c r="W3" s="13"/>
+      <c r="X3" s="13"/>
+      <c r="Y3" s="13"/>
+      <c r="Z3" s="13"/>
+      <c r="AA3" s="13"/>
+      <c r="AB3" s="13"/>
+      <c r="AC3" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="AD3" s="13"/>
+      <c r="AE3" s="13"/>
+      <c r="AF3" s="13"/>
+      <c r="AG3" s="13"/>
+      <c r="AH3" s="13"/>
+      <c r="AI3" s="13"/>
+      <c r="AJ3" s="13"/>
+      <c r="AK3" s="13"/>
+      <c r="AL3" s="13"/>
+      <c r="AM3" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="AN3" s="13"/>
+      <c r="AO3" s="13"/>
+      <c r="AP3" s="13"/>
+      <c r="AQ3" s="13"/>
+      <c r="AR3" s="13"/>
+      <c r="AS3" s="13"/>
+      <c r="AT3" s="13"/>
+      <c r="AU3" s="13"/>
+      <c r="AV3" s="13"/>
+    </row>
+    <row r="4" spans="1:48">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1">
-        <v>6</v>
-      </c>
-      <c r="H1">
+      <c r="H4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="O4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1">
+      <c r="P4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1">
+      <c r="Q4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1">
+      <c r="R4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1">
+      <c r="S4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1">
+      <c r="T4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1">
+      <c r="U4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1">
+      <c r="V4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1">
+      <c r="W4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R1">
-        <v>17</v>
-      </c>
-      <c r="S1" s="1">
-        <v>18</v>
-      </c>
-      <c r="T1">
-        <v>19</v>
-      </c>
-      <c r="U1" s="1">
-        <v>20</v>
-      </c>
-      <c r="V1">
-        <v>21</v>
-      </c>
-      <c r="W1" s="1">
-        <v>22</v>
-      </c>
-      <c r="X1">
-        <v>23</v>
+      <c r="X4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AC4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AG4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AH4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AJ4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AK4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AL4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AM4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="AO4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="AP4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="AQ4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AR4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="AS4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AT4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AU4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AV4" s="6" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
-      <c r="C2" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13"/>
-      <c r="T2" s="13"/>
-      <c r="U2" s="13"/>
-      <c r="V2" s="13"/>
-      <c r="W2" s="13"/>
-      <c r="X2" s="13"/>
+    <row r="5" spans="1:48">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <v>1</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
+      </c>
+      <c r="T5">
+        <v>1</v>
+      </c>
+      <c r="U5">
+        <v>1</v>
+      </c>
+      <c r="V5">
+        <v>1</v>
+      </c>
+      <c r="W5">
+        <v>1</v>
+      </c>
+      <c r="X5">
+        <v>1</v>
+      </c>
+      <c r="Y5">
+        <v>1</v>
+      </c>
+      <c r="Z5">
+        <v>1</v>
+      </c>
+      <c r="AA5">
+        <v>1</v>
+      </c>
+      <c r="AB5">
+        <v>1</v>
+      </c>
+      <c r="AC5">
+        <v>1</v>
+      </c>
+      <c r="AD5">
+        <v>1</v>
+      </c>
+      <c r="AE5">
+        <v>1</v>
+      </c>
+      <c r="AF5">
+        <v>1</v>
+      </c>
+      <c r="AG5">
+        <v>1</v>
+      </c>
+      <c r="AH5">
+        <v>1</v>
+      </c>
+      <c r="AI5">
+        <v>1</v>
+      </c>
+      <c r="AJ5">
+        <v>1</v>
+      </c>
+      <c r="AK5">
+        <v>1</v>
+      </c>
+      <c r="AL5">
+        <v>1</v>
+      </c>
+      <c r="AM5">
+        <v>1</v>
+      </c>
+      <c r="AN5">
+        <v>1</v>
+      </c>
+      <c r="AO5">
+        <v>1</v>
+      </c>
+      <c r="AP5">
+        <v>1</v>
+      </c>
+      <c r="AQ5">
+        <v>1</v>
+      </c>
+      <c r="AR5">
+        <v>1</v>
+      </c>
+      <c r="AS5">
+        <v>1</v>
+      </c>
+      <c r="AT5">
+        <v>1</v>
+      </c>
+      <c r="AU5">
+        <v>1</v>
+      </c>
+      <c r="AV5">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:24">
-      <c r="C3" s="1"/>
-      <c r="D3" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="14"/>
-      <c r="S3" s="14"/>
-      <c r="T3" s="14"/>
-      <c r="U3" s="14"/>
-      <c r="V3" s="14"/>
-      <c r="W3" s="14"/>
-      <c r="X3" s="14"/>
+    <row r="6" spans="1:48">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>2</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
+      <c r="J6">
+        <v>2</v>
+      </c>
+      <c r="K6">
+        <v>2</v>
+      </c>
+      <c r="L6">
+        <v>2</v>
+      </c>
+      <c r="M6">
+        <v>2</v>
+      </c>
+      <c r="N6">
+        <v>2</v>
+      </c>
+      <c r="O6">
+        <v>2</v>
+      </c>
+      <c r="P6">
+        <v>2</v>
+      </c>
+      <c r="Q6">
+        <v>2</v>
+      </c>
+      <c r="R6">
+        <v>2</v>
+      </c>
+      <c r="S6">
+        <v>2</v>
+      </c>
+      <c r="T6">
+        <v>2</v>
+      </c>
+      <c r="U6">
+        <v>2</v>
+      </c>
+      <c r="V6">
+        <v>2</v>
+      </c>
+      <c r="W6">
+        <v>2</v>
+      </c>
+      <c r="X6">
+        <v>2</v>
+      </c>
+      <c r="Y6">
+        <v>2</v>
+      </c>
+      <c r="Z6">
+        <v>2</v>
+      </c>
+      <c r="AA6">
+        <v>2</v>
+      </c>
+      <c r="AB6">
+        <v>2</v>
+      </c>
+      <c r="AC6">
+        <v>2</v>
+      </c>
+      <c r="AD6">
+        <v>2</v>
+      </c>
+      <c r="AE6">
+        <v>2</v>
+      </c>
+      <c r="AF6">
+        <v>2</v>
+      </c>
+      <c r="AG6">
+        <v>2</v>
+      </c>
+      <c r="AH6">
+        <v>2</v>
+      </c>
+      <c r="AI6">
+        <v>2</v>
+      </c>
+      <c r="AJ6">
+        <v>2</v>
+      </c>
+      <c r="AK6">
+        <v>2</v>
+      </c>
+      <c r="AL6">
+        <v>2</v>
+      </c>
+      <c r="AM6">
+        <v>2</v>
+      </c>
+      <c r="AN6">
+        <v>2</v>
+      </c>
+      <c r="AO6">
+        <v>2</v>
+      </c>
+      <c r="AP6">
+        <v>2</v>
+      </c>
+      <c r="AQ6">
+        <v>2</v>
+      </c>
+      <c r="AR6">
+        <v>2</v>
+      </c>
+      <c r="AS6">
+        <v>2</v>
+      </c>
+      <c r="AT6">
+        <v>2</v>
+      </c>
+      <c r="AU6">
+        <v>2</v>
+      </c>
+      <c r="AV6">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:24">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="R4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="S4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="T4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="U4" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="V4" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="W4" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="X4" s="7" t="s">
-        <v>17</v>
+    <row r="7" spans="1:48">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <v>3</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+      <c r="J7">
+        <v>3</v>
+      </c>
+      <c r="K7">
+        <v>3</v>
+      </c>
+      <c r="L7">
+        <v>3</v>
+      </c>
+      <c r="M7">
+        <v>3</v>
+      </c>
+      <c r="N7">
+        <v>3</v>
+      </c>
+      <c r="O7">
+        <v>3</v>
+      </c>
+      <c r="P7">
+        <v>3</v>
+      </c>
+      <c r="Q7">
+        <v>3</v>
+      </c>
+      <c r="R7">
+        <v>3</v>
+      </c>
+      <c r="S7">
+        <v>3</v>
+      </c>
+      <c r="T7">
+        <v>3</v>
+      </c>
+      <c r="U7">
+        <v>3</v>
+      </c>
+      <c r="V7">
+        <v>3</v>
+      </c>
+      <c r="W7">
+        <v>3</v>
+      </c>
+      <c r="X7">
+        <v>3</v>
+      </c>
+      <c r="Y7">
+        <v>3</v>
+      </c>
+      <c r="Z7">
+        <v>3</v>
+      </c>
+      <c r="AA7">
+        <v>3</v>
+      </c>
+      <c r="AB7">
+        <v>3</v>
+      </c>
+      <c r="AC7">
+        <v>3</v>
+      </c>
+      <c r="AD7">
+        <v>3</v>
+      </c>
+      <c r="AE7">
+        <v>3</v>
+      </c>
+      <c r="AF7">
+        <v>3</v>
+      </c>
+      <c r="AG7">
+        <v>3</v>
+      </c>
+      <c r="AH7">
+        <v>3</v>
+      </c>
+      <c r="AI7">
+        <v>3</v>
+      </c>
+      <c r="AJ7">
+        <v>3</v>
+      </c>
+      <c r="AK7">
+        <v>3</v>
+      </c>
+      <c r="AL7">
+        <v>3</v>
+      </c>
+      <c r="AM7">
+        <v>3</v>
+      </c>
+      <c r="AN7">
+        <v>3</v>
+      </c>
+      <c r="AO7">
+        <v>3</v>
+      </c>
+      <c r="AP7">
+        <v>3</v>
+      </c>
+      <c r="AQ7">
+        <v>3</v>
+      </c>
+      <c r="AR7">
+        <v>3</v>
+      </c>
+      <c r="AS7">
+        <v>3</v>
+      </c>
+      <c r="AT7">
+        <v>3</v>
+      </c>
+      <c r="AU7">
+        <v>3</v>
+      </c>
+      <c r="AV7">
+        <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="9"/>
-      <c r="S5" s="10"/>
-      <c r="T5" s="11"/>
-      <c r="U5" s="12"/>
-      <c r="V5" s="12"/>
-      <c r="W5" s="12"/>
-      <c r="X5" s="12"/>
-    </row>
-    <row r="6" spans="1:24">
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="9"/>
-      <c r="S6" s="10"/>
-      <c r="T6" s="11"/>
-      <c r="U6" s="12"/>
-      <c r="V6" s="12"/>
-      <c r="W6" s="12"/>
-      <c r="X6" s="12"/>
-    </row>
-    <row r="7" spans="1:24">
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="8"/>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="9"/>
-      <c r="R7" s="9"/>
-      <c r="S7" s="10"/>
-      <c r="T7" s="11"/>
-      <c r="U7" s="12"/>
-      <c r="V7" s="12"/>
-      <c r="W7" s="12"/>
-      <c r="X7" s="12"/>
-    </row>
-    <row r="8" spans="1:24">
-      <c r="C8" s="1"/>
+    <row r="8" spans="1:48">
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -1331,24 +1894,51 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="9"/>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="9"/>
-      <c r="S8" s="10"/>
-      <c r="T8" s="11"/>
-      <c r="U8" s="12"/>
-      <c r="V8" s="12"/>
-      <c r="W8" s="12"/>
-      <c r="X8" s="12"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="8"/>
+      <c r="U8" s="8"/>
+      <c r="V8" s="8"/>
+      <c r="W8" s="9"/>
+      <c r="X8" s="10"/>
+      <c r="Y8" s="11"/>
+      <c r="Z8" s="11"/>
+      <c r="AA8" s="11"/>
+      <c r="AB8" s="11"/>
+      <c r="AC8" s="7"/>
+      <c r="AD8" s="8"/>
+      <c r="AE8" s="8"/>
+      <c r="AF8" s="8"/>
+      <c r="AG8" s="9"/>
+      <c r="AH8" s="10"/>
+      <c r="AI8" s="11"/>
+      <c r="AJ8" s="11"/>
+      <c r="AK8" s="11"/>
+      <c r="AL8" s="11"/>
+      <c r="AM8" s="7"/>
+      <c r="AN8" s="8"/>
+      <c r="AO8" s="8"/>
+      <c r="AP8" s="8"/>
+      <c r="AQ8" s="9"/>
+      <c r="AR8" s="10"/>
+      <c r="AS8" s="11"/>
+      <c r="AT8" s="11"/>
+      <c r="AU8" s="11"/>
+      <c r="AV8" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="C2:X2"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="H3:N3"/>
-    <mergeCell ref="O3:X3"/>
+  <mergeCells count="6">
+    <mergeCell ref="D2:AB2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="H3:R3"/>
+    <mergeCell ref="S3:AB3"/>
+    <mergeCell ref="AC3:AL3"/>
+    <mergeCell ref="AM3:AV3"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>